<commit_message>
Updates line for LWCF to repair query
</commit_message>
<xml_diff>
--- a/gatsby-site/src/data-graphql/federal_disbursements.xlsx
+++ b/gatsby-site/src/data-graphql/federal_disbursements.xlsx
@@ -36,9 +36,6 @@
     <t>Offshore</t>
   </si>
   <si>
-    <t>Land &amp; Water Conservation Fund</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Historic Preservation</t>
+  </si>
+  <si>
+    <t>Land &amp; Water Conservation</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -452,7 +452,7 @@
         <v>2014</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -466,7 +466,7 @@
         <v>2014</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -480,7 +480,7 @@
         <v>2014</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -494,7 +494,7 @@
         <v>2014</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -508,10 +508,10 @@
         <v>2014</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>1146119619</v>
@@ -522,10 +522,10 @@
         <v>2014</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>194422815.69999999</v>
@@ -536,10 +536,10 @@
         <v>2014</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
         <v>1766192707</v>
@@ -550,10 +550,10 @@
         <v>2014</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
         <v>2187978477</v>
@@ -564,10 +564,10 @@
         <v>2014</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
         <v>551361445.39999998</v>
@@ -578,10 +578,10 @@
         <v>2014</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2">
         <v>34101233.450000003</v>
@@ -592,10 +592,10 @@
         <v>2014</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2">
         <v>877818.12</v>
@@ -606,10 +606,10 @@
         <v>2014</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2">
         <v>3362351.09</v>
@@ -620,10 +620,10 @@
         <v>2014</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2">
         <v>4297873.41</v>
@@ -634,10 +634,10 @@
         <v>2014</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2">
         <v>625237.05000000005</v>
@@ -648,7 +648,7 @@
         <v>2015</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -662,7 +662,7 @@
         <v>2015</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -676,7 +676,7 @@
         <v>2015</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -690,7 +690,7 @@
         <v>2015</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -704,10 +704,10 @@
         <v>2015</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="2">
         <v>852729350.89999998</v>
@@ -718,10 +718,10 @@
         <v>2015</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="2">
         <v>153527706.69999999</v>
@@ -732,10 +732,10 @@
         <v>2015</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="2">
         <v>1398152075</v>
@@ -746,10 +746,10 @@
         <v>2015</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="2">
         <v>1814559611</v>
@@ -760,10 +760,10 @@
         <v>2015</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="2">
         <v>430430343.80000001</v>
@@ -774,10 +774,10 @@
         <v>2015</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="2">
         <v>22146231.09</v>
@@ -788,10 +788,10 @@
         <v>2015</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" s="2">
         <v>95097.14</v>
@@ -802,10 +802,10 @@
         <v>2015</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="2">
         <v>1399279.23</v>
@@ -816,10 +816,10 @@
         <v>2015</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="2">
         <v>2441209.0299999998</v>
@@ -830,10 +830,10 @@
         <v>2015</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" s="2">
         <v>1232665.94</v>
@@ -844,7 +844,7 @@
         <v>2016</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -858,7 +858,7 @@
         <v>2016</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -872,7 +872,7 @@
         <v>2016</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -886,10 +886,10 @@
         <v>2016</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" s="2">
         <v>560416155.20000005</v>
@@ -900,10 +900,10 @@
         <v>2016</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" s="2">
         <v>91256204.900000006</v>
@@ -914,10 +914,10 @@
         <v>2016</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" s="2">
         <v>1009078895</v>
@@ -928,10 +928,10 @@
         <v>2016</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D36" s="2">
         <v>1316110458</v>
@@ -942,10 +942,10 @@
         <v>2016</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37" s="2">
         <v>336570856.30000001</v>
@@ -956,10 +956,10 @@
         <v>2016</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" s="2">
         <v>10774005.140000001</v>
@@ -970,10 +970,10 @@
         <v>2016</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39" s="2">
         <v>342654.53</v>
@@ -984,10 +984,10 @@
         <v>2016</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" s="2">
         <v>2352673.85</v>
@@ -998,10 +998,10 @@
         <v>2016</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" s="2">
         <v>314205.13</v>
@@ -1012,10 +1012,10 @@
         <v>2016</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42" s="2">
         <v>1370611.67</v>
@@ -1026,7 +1026,7 @@
         <v>2017</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -1040,7 +1040,7 @@
         <v>2017</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -1052,7 +1052,7 @@
         <v>2017</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -1066,7 +1066,7 @@
         <v>2017</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -1080,10 +1080,10 @@
         <v>2017</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D47" s="2">
         <v>675788643.29999995</v>
@@ -1094,10 +1094,10 @@
         <v>2017</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D48" s="2">
         <v>111303696.59999999</v>
@@ -1108,10 +1108,10 @@
         <v>2017</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D49" s="2">
         <v>1142376549</v>
@@ -1122,10 +1122,10 @@
         <v>2017</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50" s="2">
         <v>1427205064</v>
@@ -1136,10 +1136,10 @@
         <v>2017</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D51" s="2">
         <v>496239191.89999998</v>
@@ -1150,10 +1150,10 @@
         <v>2017</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D52" s="2">
         <v>10320922.99</v>
@@ -1164,10 +1164,10 @@
         <v>2017</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53" s="2">
         <v>66982984.719999999</v>
@@ -1178,10 +1178,10 @@
         <v>2017</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D54" s="2">
         <v>77617720.030000001</v>
@@ -1192,10 +1192,10 @@
         <v>2017</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D55" s="2">
         <v>957032.29</v>
@@ -1206,10 +1206,10 @@
         <v>2017</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D56" s="2">
         <v>267931822.90000001</v>
@@ -1220,7 +1220,7 @@
         <v>2018</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>4</v>
@@ -1234,7 +1234,7 @@
         <v>2018</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>4</v>
@@ -1248,7 +1248,7 @@
         <v>2018</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>4</v>
@@ -1262,7 +1262,7 @@
         <v>2018</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>4</v>
@@ -1276,10 +1276,10 @@
         <v>2018</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D61" s="2">
         <v>1022539457</v>
@@ -1290,10 +1290,10 @@
         <v>2018</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D62" s="2">
         <v>163170753</v>
@@ -1304,10 +1304,10 @@
         <v>2018</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D63" s="2">
         <v>1221259347</v>
@@ -1318,10 +1318,10 @@
         <v>2018</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D64" s="2">
         <v>1577829653</v>
@@ -1332,10 +1332,10 @@
         <v>2018</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D65" s="2">
         <v>411828484.5</v>
@@ -1346,10 +1346,10 @@
         <v>2018</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D66" s="2">
         <v>16204907.98</v>
@@ -1360,10 +1360,10 @@
         <v>2018</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D67" s="2">
         <v>76357901.969999999</v>
@@ -1374,10 +1374,10 @@
         <v>2018</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D68" s="2">
         <v>187988933.09999999</v>
@@ -1388,10 +1388,10 @@
         <v>2018</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D69" s="2">
         <v>309064093.10000002</v>

</xml_diff>

<commit_message>
Corrects one data value and adds punctuation to disbursements sentence
</commit_message>
<xml_diff>
--- a/gatsby-site/src/data-graphql/federal_disbursements.xlsx
+++ b/gatsby-site/src/data-graphql/federal_disbursements.xlsx
@@ -89,7 +89,9 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +139,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,8 +425,8 @@
   </sheetPr>
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1047,9 @@
       <c r="C44" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5">
+        <v>891828225</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
@@ -1399,5 +1403,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trying again with the correct file
</commit_message>
<xml_diff>
--- a/gatsby-site/src/data-graphql/federal_disbursements.xlsx
+++ b/gatsby-site/src/data-graphql/federal_disbursements.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsobr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcolmj\Documents\GitHub\doi-extractives-data\gatsby-site\src\data-graphql\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="15">
   <si>
     <t>Year</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land &amp; Water Conservation </t>
   </si>
 </sst>
 </file>
@@ -399,17 +396,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="2" customWidth="1"/>
     <col min="3" max="4" width="18" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2009</v>
       </c>
@@ -437,7 +436,7 @@
         <v>449462056.69999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2009</v>
       </c>
@@ -451,7 +450,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2009</v>
       </c>
@@ -465,7 +464,7 @@
         <v>909915.47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2009</v>
       </c>
@@ -479,7 +478,7 @@
         <v>898090084.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2009</v>
       </c>
@@ -493,7 +492,7 @@
         <v>1454102007</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2009</v>
       </c>
@@ -507,7 +506,7 @@
         <v>54651967.960000008</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2009</v>
       </c>
@@ -521,7 +520,7 @@
         <v>25240041.039999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2009</v>
       </c>
@@ -535,7 +534,7 @@
         <v>1915191159.8200002</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2009</v>
       </c>
@@ -549,7 +548,7 @@
         <v>3639656.61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2009</v>
       </c>
@@ -563,7 +562,7 @@
         <v>5093231404.3900003</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2009</v>
       </c>
@@ -577,7 +576,7 @@
         <v>640202103</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2010</v>
       </c>
@@ -591,7 +590,7 @@
         <v>407559568.80000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2010</v>
       </c>
@@ -605,7 +604,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2010</v>
       </c>
@@ -619,7 +618,7 @@
         <v>288653.84000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2010</v>
       </c>
@@ -633,7 +632,7 @@
         <v>898711346.20000005</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2010</v>
       </c>
@@ -647,7 +646,7 @@
         <v>1363951779</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2010</v>
       </c>
@@ -661,7 +660,7 @@
         <v>46786549.410000004</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2010</v>
       </c>
@@ -675,7 +674,7 @@
         <v>2729743.6800000006</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2010</v>
       </c>
@@ -689,7 +688,7 @@
         <v>1782709381.6700001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2010</v>
       </c>
@@ -703,7 +702,7 @@
         <v>1154615.3500000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2010</v>
       </c>
@@ -717,7 +716,7 @@
         <v>3907952116.6500001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2010</v>
       </c>
@@ -731,7 +730,7 @@
         <v>607810866</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2011</v>
       </c>
@@ -745,7 +744,7 @@
         <v>538344246.89999998</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2011</v>
       </c>
@@ -759,7 +758,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2011</v>
       </c>
@@ -773,7 +772,7 @@
         <v>104666.34</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2011</v>
       </c>
@@ -787,7 +786,7 @@
         <v>891870938.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2011</v>
       </c>
@@ -801,7 +800,7 @@
         <v>1532623172</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2011</v>
       </c>
@@ -815,7 +814,7 @@
         <v>40996495.630000003</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>2011</v>
       </c>
@@ -829,7 +828,7 @@
         <v>865961.51</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>2011</v>
       </c>
@@ -843,7 +842,7 @@
         <v>1957196095.8900001</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>2011</v>
       </c>
@@ -857,7 +856,7 @@
         <v>418665.35</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2011</v>
       </c>
@@ -871,7 +870,7 @@
         <v>5394172814.6499996</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>2011</v>
       </c>
@@ -885,7 +884,7 @@
         <v>655649401</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>2012</v>
       </c>
@@ -899,7 +898,7 @@
         <v>717556925.10000002</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>2012</v>
       </c>
@@ -913,7 +912,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2012</v>
       </c>
@@ -927,7 +926,7 @@
         <v>104666.34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2012</v>
       </c>
@@ -941,7 +940,7 @@
         <v>897036446.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2012</v>
       </c>
@@ -955,7 +954,7 @@
         <v>205493260.06999999</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2012</v>
       </c>
@@ -969,7 +968,7 @@
         <v>214991515.77000001</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2012</v>
       </c>
@@ -983,7 +982,7 @@
         <v>1646314405</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>2012</v>
       </c>
@@ -997,7 +996,7 @@
         <v>36658094.600000001</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>2012</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>313999.01</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>2012</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>2088316004.8099999</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>2012</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>635463.24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>2012</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>5705170929.41998</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>2012</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>489059561.72999799</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>2013</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>932956397.20000005</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>2013</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>2013</v>
       </c>
@@ -1109,7 +1108,7 @@
         <v>1543777.36</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>2013</v>
       </c>
@@ -1123,7 +1122,7 @@
         <v>894036704.94999993</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>2013</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>228785871.94999999</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2013</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>168544944.88</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>2013</v>
       </c>
@@ -1165,7 +1164,7 @@
         <v>1592181337</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>2013</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>40641441.630000003</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>2013</v>
       </c>
@@ -1193,7 +1192,7 @@
         <v>297985.05000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>2013</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>1964029388.52</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>2013</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>539623.81999999995</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>2013</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>7760122579.2299995</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>2013</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>490695402.18000001</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>2014</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>1146119618.6800001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>2014</v>
       </c>
@@ -1277,7 +1276,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>2014</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>877818.12</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>2014</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>894379939.88</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>2014</v>
       </c>
@@ -1319,7 +1318,7 @@
         <v>220518478.92000002</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>2014</v>
       </c>
@@ -1333,7 +1332,7 @@
         <v>194422815.68000001</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>2014</v>
       </c>
@@ -1347,7 +1346,7 @@
         <v>1766192706.99</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>2014</v>
       </c>
@@ -1361,7 +1360,7 @@
         <v>34101233.449999996</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>2014</v>
       </c>
@@ -1375,7 +1374,7 @@
         <v>4297873.410000002</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>2014</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>2187978477.289999</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>2014</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>625237.05000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>2014</v>
       </c>
@@ -1417,7 +1416,7 @@
         <v>6303362577.8599997</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>2014</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>551361445.35000098</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>2015</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>852729350.94000006</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>2015</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>2015</v>
       </c>
@@ -1473,12 +1472,12 @@
         <v>95097.14</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>2015</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>7</v>
@@ -1487,7 +1486,7 @@
         <v>888459462.86000001</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>2015</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>200739928.84999999</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>2015</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>153527706.74000001</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>2015</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>1398152074.75</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>2015</v>
       </c>
@@ -1543,7 +1542,7 @@
         <v>22146231.09</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>2015</v>
       </c>
@@ -1557,7 +1556,7 @@
         <v>2441209.0300000003</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>2015</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>1814559610.5500021</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>2015</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>1232665.94</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>2015</v>
       </c>
@@ -1599,7 +1598,7 @@
         <v>3962702079.6599998</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>2015</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>430430343.81</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>2016</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>560416155.14999998</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>2016</v>
       </c>
@@ -1641,12 +1640,12 @@
         <v>342654.53</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>2016</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>7</v>
@@ -1655,7 +1654,7 @@
         <v>883627822.51999998</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>2016</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>158644486.10999998</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>2016</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>91256204.899999902</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>2016</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>1009078894.55999</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>2016</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>10774005.139999999</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>2016</v>
       </c>
@@ -1725,7 +1724,7 @@
         <v>314205.12999999983</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>2016</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>1316110457.940001</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>2016</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>1370611.67</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>2016</v>
       </c>
@@ -1767,7 +1766,7 @@
         <v>1865028729.49</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>2016</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>336570856.33999997</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>2017</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>675788643.3400023</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>2017</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>2017</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>66982984.720000036</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>2017</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>891828225.00000024</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>2017</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>122238329.06000003</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>2017</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>111303696.5900002</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>2017</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>1142376548.9999981</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>2017</v>
       </c>
@@ -1893,7 +1892,7 @@
         <v>10320922.99</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>2017</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>957032.2899999998</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>2017</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>1427205063.670001</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>2017</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>267931822.86000061</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>2017</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>1748637163.690006</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>2017</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>496239191.86999989</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>2018</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>1022539457.2899991</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>2018</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>2018</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>76357901.970000029</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>2018</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>893887297</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>2018</v>
       </c>
@@ -2033,7 +2032,7 @@
         <v>116875634.66</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>2018</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>163170752.99000001</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>2018</v>
       </c>
@@ -2061,7 +2060,7 @@
         <v>1221259347.2999983</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>2018</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>16204907.979999999</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>2018</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>187988933.10000002</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>2018</v>
       </c>
@@ -2103,7 +2102,7 @@
         <v>1577829653</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>2018</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>309064093.10999995</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>2018</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>2789421770.9399981</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>2018</v>
       </c>

</xml_diff>